<commit_message>
feat: se implementaron mejoras técnicas y visualescomo agregar 10 audiencias más, quitar el widget de fecha, colocar un seleccionar archivo en los dropdowm, entre otros
</commit_message>
<xml_diff>
--- a/archivos_creados/prueba.xlsx
+++ b/archivos_creados/prueba.xlsx
@@ -853,52 +853,6 @@
     </indexedColors>
   </colors>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <twoCellAnchor editAs="oneCell">
-    <from>
-      <col>0</col>
-      <colOff>57728</colOff>
-      <row>4</row>
-      <rowOff>138546</rowOff>
-    </from>
-    <to>
-      <col>0</col>
-      <colOff>638753</colOff>
-      <row>7</row>
-      <rowOff>14900</rowOff>
-    </to>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="2" name="Imagen 1"/>
-        <cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </cNvPicPr>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:xfrm>
-          <a:off x="57728" y="889001"/>
-          <a:ext cx="581025" cy="603717"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </spPr>
-    </pic>
-    <clientData/>
-  </twoCellAnchor>
-</wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1582,22 +1536,50 @@
       <c r="A14" s="8" t="n">
         <v>4</v>
       </c>
-      <c r="B14" s="9" t="n"/>
-      <c r="C14" s="5" t="n"/>
-      <c r="D14" s="6" t="n"/>
-      <c r="E14" s="7" t="n"/>
-      <c r="F14" s="4" t="n"/>
-      <c r="G14" s="4" t="n"/>
-      <c r="H14" s="18" t="n"/>
-      <c r="I14" s="18" t="n"/>
-      <c r="J14" s="18" t="n"/>
-      <c r="K14" s="18" t="n"/>
-      <c r="L14" s="18" t="n"/>
-      <c r="M14" s="18" t="n"/>
-      <c r="N14" s="18" t="n"/>
-      <c r="O14" s="18" t="n"/>
-      <c r="P14" s="18" t="n"/>
-      <c r="Q14" s="22" t="n"/>
+      <c r="B14" s="9" t="inlineStr">
+        <is>
+          <t>kjjkjkljk</t>
+        </is>
+      </c>
+      <c r="C14" s="5" t="inlineStr">
+        <is>
+          <t>Audiencia preparatoria</t>
+        </is>
+      </c>
+      <c r="D14" s="6" t="inlineStr">
+        <is>
+          <t>11/07/2024</t>
+        </is>
+      </c>
+      <c r="E14" s="7" t="inlineStr">
+        <is>
+          <t>12:21</t>
+        </is>
+      </c>
+      <c r="F14" s="4" t="inlineStr">
+        <is>
+          <t>sjkadskljdasd</t>
+        </is>
+      </c>
+      <c r="G14" s="4" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
+      <c r="H14" s="18" t="inlineStr"/>
+      <c r="I14" s="18" t="inlineStr"/>
+      <c r="J14" s="18" t="inlineStr"/>
+      <c r="K14" s="18" t="inlineStr"/>
+      <c r="L14" s="18" t="inlineStr"/>
+      <c r="M14" s="18" t="inlineStr"/>
+      <c r="N14" s="18" t="inlineStr"/>
+      <c r="O14" s="18" t="inlineStr"/>
+      <c r="P14" s="18" t="inlineStr"/>
+      <c r="Q14" s="22" t="inlineStr">
+        <is>
+          <t>erdaaa</t>
+        </is>
+      </c>
     </row>
     <row r="15" ht="150" customHeight="1">
       <c r="A15" s="8" t="n">
@@ -3623,7 +3605,7 @@
       <c r="E111" s="21" t="n"/>
       <c r="F111" s="21" t="n"/>
       <c r="G111" s="33" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H111" s="10" t="inlineStr">
         <is>
@@ -3697,6 +3679,5 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" scale="33"/>
-  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>